<commit_message>
Added 2024 data and run estimates.
Quite a bit of time spent deciding how to handle 2024 Lake Creek sonar which was likely contaminated with sockeye after 7/10 (last few days). The version here uses Nick's judgement to remove fish in obvious groups after 7/10 (3453 total Chinook). I had run an earlier version using only fish > 750mm mef after 7/10 (2685 total Chinook) which resulted in a substantially smaller estimate of Yentna abundances (~7.8K). That said it looks like there were large numbers of smaller Chinook passing after 7/10 so Nick felt the estimate included is more reliable. Tried to move the 2024 html to the docs folder so it will show up in github pages… fingers crossed… and reran the 2023 qmd so I’d have a copy of the html in the directory.
</commit_message>
<xml_diff>
--- a/data-raw/SusitnaEG Ha_post95.xlsx
+++ b/data-raw/SusitnaEG Ha_post95.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\SusitnaEG\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\RTS\Reimer\SusitnaEG\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88E5694-7139-49A6-ABC0-94252DF502B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B85904-9588-41A2-A3FE-DB542E88AE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-14055" windowWidth="21840" windowHeight="37920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="su_har" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="837">
   <si>
     <t>Susitna Area Chinook Harvest</t>
   </si>
@@ -2546,6 +2546,9 @@
   </si>
   <si>
     <t>No harvest per 11/22/22 email from Nick</t>
+  </si>
+  <si>
+    <t>No harvest per 1/10/2023 email from Nick</t>
   </si>
 </sst>
 </file>
@@ -2852,7 +2855,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3944,7 +3947,45 @@
         <v>834</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2024</v>
+      </c>
+      <c r="B33" s="10">
+        <v>0</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+      <c r="E33" s="10">
+        <v>0</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0</v>
+      </c>
+      <c r="I33" s="10">
+        <v>0</v>
+      </c>
+      <c r="J33" s="10">
+        <v>0</v>
+      </c>
+      <c r="K33" s="10">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>14</v>
       </c>

</xml_diff>